<commit_message>
fix | plantilla excel
</commit_message>
<xml_diff>
--- a/public/templates/PlantillaDocumentos.xlsx
+++ b/public/templates/PlantillaDocumentos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat1\Desktop\EXCELS IMPORTACION DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA4356-E773-454A-BA88-C028E976DCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C25F984-5AFD-4A6E-BAB0-5ACC87044C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cabecera" sheetId="1" r:id="rId1"/>
     <sheet name="Detalle" sheetId="2" r:id="rId2"/>
-    <sheet name="TIPOS-LISTAS" sheetId="4" r:id="rId3"/>
+    <sheet name="TIPOS-LISTAS" sheetId="4" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_1____Factura">#REF!</definedName>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>